<commit_message>
Minor edits in datasets. Syntax debugged until ACCall variable computation.
</commit_message>
<xml_diff>
--- a/Experiment_3/qualtrics_to_matlab.xlsx
+++ b/Experiment_3/qualtrics_to_matlab.xlsx
@@ -543,7 +543,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -551,13 +551,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -569,15 +593,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -883,8 +920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AP56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="AK5" workbookViewId="0">
+      <selection activeCell="AM27" sqref="AM27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -914,7 +951,7 @@
     <col min="30" max="30" width="59.42578125" bestFit="1" customWidth="1"/>
     <col min="31" max="37" width="71.42578125" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="59.85546875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="81.140625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="95.28515625" style="3" customWidth="1"/>
     <col min="40" max="40" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="16.28515625" bestFit="1" customWidth="1"/>
@@ -1035,7 +1072,7 @@
       <c r="AL1" t="s">
         <v>40</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AM1" s="3" t="s">
         <v>41</v>
       </c>
       <c r="AN1" t="s">
@@ -1154,6 +1191,7 @@
       <c r="AL2">
         <v>5</v>
       </c>
+      <c r="AM2" s="4"/>
       <c r="AN2" t="s">
         <v>46</v>
       </c>
@@ -1164,7 +1202,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:42" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>48</v>
       </c>
@@ -1267,7 +1305,7 @@
       <c r="AL3">
         <v>5</v>
       </c>
-      <c r="AM3" t="s">
+      <c r="AM3" s="4" t="s">
         <v>50</v>
       </c>
       <c r="AN3" t="s">
@@ -1386,6 +1424,7 @@
       <c r="AL4">
         <v>2</v>
       </c>
+      <c r="AM4" s="4"/>
       <c r="AN4" t="s">
         <v>46</v>
       </c>
@@ -1502,7 +1541,7 @@
       <c r="AL5">
         <v>4</v>
       </c>
-      <c r="AM5" t="s">
+      <c r="AM5" s="4" t="s">
         <v>54</v>
       </c>
       <c r="AN5" t="s">
@@ -1621,6 +1660,7 @@
       <c r="AL6">
         <v>4</v>
       </c>
+      <c r="AM6" s="4"/>
       <c r="AN6" t="s">
         <v>46</v>
       </c>
@@ -1737,7 +1777,7 @@
       <c r="AL7">
         <v>5</v>
       </c>
-      <c r="AM7" t="s">
+      <c r="AM7" s="4" t="s">
         <v>57</v>
       </c>
       <c r="AN7" t="s">
@@ -1856,7 +1896,7 @@
       <c r="AL8">
         <v>3</v>
       </c>
-      <c r="AM8" t="s">
+      <c r="AM8" s="4" t="s">
         <v>59</v>
       </c>
       <c r="AN8" t="s">
@@ -1869,7 +1909,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:42" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>60</v>
       </c>
@@ -1975,7 +2015,7 @@
       <c r="AL9">
         <v>2</v>
       </c>
-      <c r="AM9" t="s">
+      <c r="AM9" s="5" t="s">
         <v>61</v>
       </c>
       <c r="AN9" t="s">
@@ -2094,7 +2134,7 @@
       <c r="AL10">
         <v>2</v>
       </c>
-      <c r="AM10" t="s">
+      <c r="AM10" s="4" t="s">
         <v>63</v>
       </c>
       <c r="AN10" t="s">
@@ -2107,7 +2147,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:42" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>64</v>
       </c>
@@ -2213,7 +2253,7 @@
       <c r="AL11">
         <v>4</v>
       </c>
-      <c r="AM11" t="s">
+      <c r="AM11" s="4" t="s">
         <v>66</v>
       </c>
       <c r="AN11" t="s">
@@ -2226,7 +2266,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="12" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:42" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>67</v>
       </c>
@@ -2332,7 +2372,7 @@
       <c r="AL12">
         <v>3</v>
       </c>
-      <c r="AM12" t="s">
+      <c r="AM12" s="4" t="s">
         <v>68</v>
       </c>
       <c r="AN12" t="s">
@@ -2345,7 +2385,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="13" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:42" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>69</v>
       </c>
@@ -2451,7 +2491,7 @@
       <c r="AL13">
         <v>5</v>
       </c>
-      <c r="AM13" t="s">
+      <c r="AM13" s="4" t="s">
         <v>70</v>
       </c>
       <c r="AN13" t="s">
@@ -2570,7 +2610,7 @@
       <c r="AL14">
         <v>4</v>
       </c>
-      <c r="AM14" t="s">
+      <c r="AM14" s="4" t="s">
         <v>72</v>
       </c>
       <c r="AN14" t="s">
@@ -2583,7 +2623,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="15" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:42" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>73</v>
       </c>
@@ -2689,7 +2729,7 @@
       <c r="AL15">
         <v>2</v>
       </c>
-      <c r="AM15" t="s">
+      <c r="AM15" s="4" t="s">
         <v>75</v>
       </c>
       <c r="AN15" t="s">
@@ -2702,7 +2742,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="16" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:42" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>76</v>
       </c>
@@ -2808,7 +2848,7 @@
       <c r="AL16">
         <v>4</v>
       </c>
-      <c r="AM16" t="s">
+      <c r="AM16" s="4" t="s">
         <v>78</v>
       </c>
       <c r="AN16" t="s">
@@ -2927,7 +2967,7 @@
       <c r="AL17">
         <v>2</v>
       </c>
-      <c r="AM17" t="s">
+      <c r="AM17" s="4" t="s">
         <v>80</v>
       </c>
       <c r="AN17" t="s">
@@ -3046,7 +3086,7 @@
       <c r="AL18">
         <v>4</v>
       </c>
-      <c r="AM18" t="s">
+      <c r="AM18" s="4" t="s">
         <v>82</v>
       </c>
       <c r="AN18" t="s">
@@ -3165,7 +3205,7 @@
       <c r="AL19">
         <v>1</v>
       </c>
-      <c r="AM19" t="s">
+      <c r="AM19" s="4" t="s">
         <v>84</v>
       </c>
       <c r="AN19" t="s">
@@ -3178,7 +3218,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="20" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:42" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>85</v>
       </c>
@@ -3284,7 +3324,7 @@
       <c r="AL20">
         <v>4</v>
       </c>
-      <c r="AM20" t="s">
+      <c r="AM20" s="4" t="s">
         <v>87</v>
       </c>
       <c r="AN20" t="s">
@@ -3297,7 +3337,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="21" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:42" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>88</v>
       </c>
@@ -3403,7 +3443,7 @@
       <c r="AL21">
         <v>1</v>
       </c>
-      <c r="AM21" t="s">
+      <c r="AM21" s="4" t="s">
         <v>89</v>
       </c>
       <c r="AN21" t="s">
@@ -3522,7 +3562,7 @@
       <c r="AL22">
         <v>2</v>
       </c>
-      <c r="AM22" t="s">
+      <c r="AM22" s="4" t="s">
         <v>91</v>
       </c>
       <c r="AN22" t="s">
@@ -3641,7 +3681,7 @@
       <c r="AL23">
         <v>3</v>
       </c>
-      <c r="AM23" t="s">
+      <c r="AM23" s="4" t="s">
         <v>93</v>
       </c>
       <c r="AN23" t="s">
@@ -3760,7 +3800,7 @@
       <c r="AL24">
         <v>2</v>
       </c>
-      <c r="AM24" t="s">
+      <c r="AM24" s="4" t="s">
         <v>95</v>
       </c>
       <c r="AN24" t="s">
@@ -3873,7 +3913,7 @@
       <c r="AL25">
         <v>5</v>
       </c>
-      <c r="AM25" t="s">
+      <c r="AM25" s="4" t="s">
         <v>97</v>
       </c>
       <c r="AN25" t="s">
@@ -3992,7 +4032,7 @@
       <c r="AL26">
         <v>1</v>
       </c>
-      <c r="AM26" t="s">
+      <c r="AM26" s="4" t="s">
         <v>99</v>
       </c>
       <c r="AN26" t="s">
@@ -4005,7 +4045,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="27" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:42" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>100</v>
       </c>
@@ -4111,7 +4151,7 @@
       <c r="AL27">
         <v>4</v>
       </c>
-      <c r="AM27" t="s">
+      <c r="AM27" s="5" t="s">
         <v>101</v>
       </c>
       <c r="AN27" t="s">
@@ -4124,7 +4164,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="28" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:42" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>102</v>
       </c>
@@ -4230,7 +4270,7 @@
       <c r="AL28">
         <v>3</v>
       </c>
-      <c r="AM28" t="s">
+      <c r="AM28" s="4" t="s">
         <v>103</v>
       </c>
       <c r="AN28" t="s">
@@ -4349,7 +4389,7 @@
       <c r="AL29">
         <v>2</v>
       </c>
-      <c r="AM29" t="s">
+      <c r="AM29" s="4" t="s">
         <v>105</v>
       </c>
       <c r="AN29" t="s">
@@ -4362,7 +4402,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="30" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:42" ht="75" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>106</v>
       </c>
@@ -4468,7 +4508,7 @@
       <c r="AL30">
         <v>2</v>
       </c>
-      <c r="AM30" t="s">
+      <c r="AM30" s="4" t="s">
         <v>107</v>
       </c>
       <c r="AN30" t="s">
@@ -4587,7 +4627,7 @@
       <c r="AL31">
         <v>4</v>
       </c>
-      <c r="AM31" t="s">
+      <c r="AM31" s="4" t="s">
         <v>109</v>
       </c>
       <c r="AN31" t="s">
@@ -4600,7 +4640,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="32" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:42" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>110</v>
       </c>
@@ -4706,7 +4746,7 @@
       <c r="AL32">
         <v>3</v>
       </c>
-      <c r="AM32" t="s">
+      <c r="AM32" s="4" t="s">
         <v>111</v>
       </c>
       <c r="AN32" t="s">
@@ -4825,7 +4865,7 @@
       <c r="AL33">
         <v>2</v>
       </c>
-      <c r="AM33" t="s">
+      <c r="AM33" s="4" t="s">
         <v>97</v>
       </c>
       <c r="AN33" t="s">
@@ -4944,7 +4984,7 @@
       <c r="AL34">
         <v>1</v>
       </c>
-      <c r="AM34" t="s">
+      <c r="AM34" s="4" t="s">
         <v>97</v>
       </c>
       <c r="AN34" t="s">
@@ -4957,7 +4997,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="35" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:42" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>114</v>
       </c>
@@ -5063,7 +5103,7 @@
       <c r="AL35">
         <v>4</v>
       </c>
-      <c r="AM35" t="s">
+      <c r="AM35" s="4" t="s">
         <v>115</v>
       </c>
       <c r="AN35" t="s">
@@ -5182,7 +5222,7 @@
       <c r="AL36">
         <v>3</v>
       </c>
-      <c r="AM36" t="s">
+      <c r="AM36" s="4" t="s">
         <v>117</v>
       </c>
       <c r="AN36" t="s">
@@ -5195,7 +5235,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="37" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:42" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>118</v>
       </c>
@@ -5301,7 +5341,7 @@
       <c r="AL37">
         <v>2</v>
       </c>
-      <c r="AM37" t="s">
+      <c r="AM37" s="4" t="s">
         <v>119</v>
       </c>
       <c r="AN37" t="s">
@@ -5420,7 +5460,7 @@
       <c r="AL38">
         <v>3</v>
       </c>
-      <c r="AM38" t="s">
+      <c r="AM38" s="4" t="s">
         <v>121</v>
       </c>
       <c r="AN38" t="s">
@@ -5433,7 +5473,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="39" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:42" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>122</v>
       </c>
@@ -5539,7 +5579,7 @@
       <c r="AL39">
         <v>3</v>
       </c>
-      <c r="AM39" t="s">
+      <c r="AM39" s="4" t="s">
         <v>123</v>
       </c>
       <c r="AN39" t="s">
@@ -5552,7 +5592,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="40" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:42" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>124</v>
       </c>
@@ -5658,7 +5698,7 @@
       <c r="AL40">
         <v>3</v>
       </c>
-      <c r="AM40" t="s">
+      <c r="AM40" s="4" t="s">
         <v>125</v>
       </c>
       <c r="AN40" t="s">
@@ -5777,7 +5817,7 @@
       <c r="AL41">
         <v>4</v>
       </c>
-      <c r="AM41" t="s">
+      <c r="AM41" s="4" t="s">
         <v>127</v>
       </c>
       <c r="AN41" t="s">
@@ -5790,7 +5830,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="42" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:42" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>128</v>
       </c>
@@ -5896,7 +5936,7 @@
       <c r="AL42">
         <v>4</v>
       </c>
-      <c r="AM42" t="s">
+      <c r="AM42" s="4" t="s">
         <v>129</v>
       </c>
       <c r="AN42" t="s">
@@ -5909,7 +5949,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="43" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:42" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>130</v>
       </c>
@@ -6015,7 +6055,7 @@
       <c r="AL43">
         <v>3</v>
       </c>
-      <c r="AM43" t="s">
+      <c r="AM43" s="4" t="s">
         <v>131</v>
       </c>
       <c r="AN43" t="s">
@@ -6134,7 +6174,7 @@
       <c r="AL44">
         <v>4</v>
       </c>
-      <c r="AM44" t="s">
+      <c r="AM44" s="4" t="s">
         <v>80</v>
       </c>
       <c r="AN44" t="s">
@@ -6253,6 +6293,7 @@
       <c r="AL45">
         <v>4</v>
       </c>
+      <c r="AM45" s="4"/>
       <c r="AN45" t="s">
         <v>46</v>
       </c>
@@ -6263,7 +6304,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="46" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:42" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>134</v>
       </c>
@@ -6369,7 +6410,7 @@
       <c r="AL46">
         <v>2</v>
       </c>
-      <c r="AM46" t="s">
+      <c r="AM46" s="4" t="s">
         <v>135</v>
       </c>
       <c r="AN46" t="s">
@@ -6382,7 +6423,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="47" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:42" ht="45" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>136</v>
       </c>
@@ -6488,7 +6529,7 @@
       <c r="AL47">
         <v>4</v>
       </c>
-      <c r="AM47" t="s">
+      <c r="AM47" s="4" t="s">
         <v>137</v>
       </c>
       <c r="AN47" t="s">
@@ -6607,6 +6648,7 @@
       <c r="AL48">
         <v>3</v>
       </c>
+      <c r="AM48" s="4"/>
       <c r="AN48" t="s">
         <v>46</v>
       </c>
@@ -6617,7 +6659,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="49" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:42" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>139</v>
       </c>
@@ -6723,7 +6765,7 @@
       <c r="AL49">
         <v>3</v>
       </c>
-      <c r="AM49" t="s">
+      <c r="AM49" s="4" t="s">
         <v>140</v>
       </c>
       <c r="AN49" t="s">
@@ -6842,7 +6884,7 @@
       <c r="AL50">
         <v>3</v>
       </c>
-      <c r="AM50" t="s">
+      <c r="AM50" s="4" t="s">
         <v>80</v>
       </c>
       <c r="AN50" t="s">
@@ -6855,7 +6897,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="51" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:42" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>142</v>
       </c>
@@ -6961,7 +7003,7 @@
       <c r="AL51">
         <v>4</v>
       </c>
-      <c r="AM51" t="s">
+      <c r="AM51" s="4" t="s">
         <v>143</v>
       </c>
       <c r="AN51" t="s">
@@ -7080,7 +7122,7 @@
       <c r="AL52">
         <v>1</v>
       </c>
-      <c r="AM52" t="s">
+      <c r="AM52" s="4" t="s">
         <v>146</v>
       </c>
       <c r="AN52" t="s">
@@ -7199,7 +7241,7 @@
       <c r="AL53">
         <v>4</v>
       </c>
-      <c r="AM53" t="s">
+      <c r="AM53" s="4" t="s">
         <v>148</v>
       </c>
       <c r="AN53" t="s">
@@ -7212,7 +7254,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="54" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:42" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>149</v>
       </c>
@@ -7318,7 +7360,7 @@
       <c r="AL54">
         <v>1</v>
       </c>
-      <c r="AM54" t="s">
+      <c r="AM54" s="4" t="s">
         <v>150</v>
       </c>
       <c r="AN54" t="s">
@@ -7437,7 +7479,7 @@
       <c r="AL55">
         <v>4</v>
       </c>
-      <c r="AM55" t="s">
+      <c r="AM55" s="4" t="s">
         <v>152</v>
       </c>
       <c r="AN55" t="s">
@@ -7556,7 +7598,7 @@
       <c r="AL56">
         <v>3</v>
       </c>
-      <c r="AM56" t="s">
+      <c r="AM56" s="4" t="s">
         <v>154</v>
       </c>
       <c r="AN56" t="s">
@@ -7571,6 +7613,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>